<commit_message>
Add to ID_Photos and add entry to TTC Members.xlsx
</commit_message>
<xml_diff>
--- a/TTC Members.xlsx
+++ b/TTC Members.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamesonhidalgo\Desktop\TTC_Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamesonhidalgo\TuTraco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7921C0-810F-46B1-ABE3-14F385820D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF88DC0-7FD3-4E9C-93A8-17E774087945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Members" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="172">
   <si>
     <t>MemberID</t>
   </si>
@@ -521,6 +521,36 @@
   </si>
   <si>
     <t>09656679642</t>
+  </si>
+  <si>
+    <t>Mauricio, Erwin T.</t>
+  </si>
+  <si>
+    <t>Brgy. Ragan Sur, Delfin Albano, Isabela</t>
+  </si>
+  <si>
+    <t>09369838311</t>
+  </si>
+  <si>
+    <t>09173115921</t>
+  </si>
+  <si>
+    <t>Yadao, Nilo J.</t>
+  </si>
+  <si>
+    <t>Tabubuca, Esher P.</t>
+  </si>
+  <si>
+    <t>Brgy. Namnama, Tumauini, Isabela</t>
+  </si>
+  <si>
+    <t>09367877815</t>
+  </si>
+  <si>
+    <t>yhadskyyadao@gmail.com</t>
+  </si>
+  <si>
+    <t>Vice Chairman, BOD</t>
   </si>
 </sst>
 </file>
@@ -1081,8 +1111,8 @@
   </sheetPr>
   <dimension ref="A1:J151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1090,7 +1120,7 @@
     <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -1467,7 +1497,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>111</v>
       </c>
@@ -1488,7 +1518,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -1512,7 +1542,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="A19" t="s">
         <v>94</v>
       </c>
@@ -1533,31 +1563,76 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>162</v>
+      </c>
       <c r="C20" s="7">
         <f>SUMIF('Capital Contributions'!A:A, A20, 'Capital Contributions'!C:C) + SUMIFS('Payment History'!C:C, 'Payment History'!A:A, A20, 'Payment History'!D:D, "*Capital Build Up*")</f>
-        <v>0</v>
-      </c>
-      <c r="D20" s="11"/>
-      <c r="F20" s="13"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+        <v>26500</v>
+      </c>
+      <c r="D20" s="11">
+        <v>29942</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" t="s">
+        <v>167</v>
+      </c>
       <c r="C21" s="7">
         <f>SUMIF('Capital Contributions'!A:A, A21, 'Capital Contributions'!C:C) + SUMIFS('Payment History'!C:C, 'Payment History'!A:A, A21, 'Payment History'!D:D, "*Capital Build Up*")</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="F21" s="13"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+        <v>22500</v>
+      </c>
+      <c r="D21" s="11">
+        <v>34565</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>166</v>
+      </c>
       <c r="C22" s="7">
         <f>SUMIF('Capital Contributions'!A:A, A22, 'Capital Contributions'!C:C) + SUMIFS('Payment History'!C:C, 'Payment History'!A:A, A22, 'Payment History'!D:D, "*Capital Build Up*")</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="11"/>
-      <c r="F22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+        <v>27000</v>
+      </c>
+      <c r="D22" s="11">
+        <v>24725</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="I22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1">
       <c r="C23" s="7">
         <f>SUMIF('Capital Contributions'!A:A, A23, 'Capital Contributions'!C:C) + SUMIFS('Payment History'!C:C, 'Payment History'!A:A, A23, 'Payment History'!D:D, "*Capital Build Up*")</f>
         <v>0</v>
@@ -1565,7 +1640,7 @@
       <c r="D23" s="11"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1">
       <c r="C24" s="7">
         <f>SUMIF('Capital Contributions'!A:A, A24, 'Capital Contributions'!C:C) + SUMIFS('Payment History'!C:C, 'Payment History'!A:A, A24, 'Payment History'!D:D, "*Capital Build Up*")</f>
         <v>0</v>
@@ -1573,7 +1648,7 @@
       <c r="D24" s="11"/>
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1">
       <c r="C25" s="7">
         <f>SUMIF('Capital Contributions'!A:A, A25, 'Capital Contributions'!C:C) + SUMIFS('Payment History'!C:C, 'Payment History'!A:A, A25, 'Payment History'!D:D, "*Capital Build Up*")</f>
         <v>0</v>
@@ -1581,37 +1656,37 @@
       <c r="D25" s="11"/>
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1">
       <c r="C26" s="7"/>
       <c r="D26" s="11"/>
       <c r="F26" s="13"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1">
       <c r="C27" s="7"/>
       <c r="D27" s="11"/>
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1">
       <c r="C28" s="7"/>
       <c r="D28" s="11"/>
       <c r="F28" s="13"/>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1">
       <c r="C29" s="7"/>
       <c r="D29" s="11"/>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1">
       <c r="C30" s="7"/>
       <c r="D30" s="11"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1">
       <c r="C31" s="7"/>
       <c r="D31" s="11"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1">
       <c r="C32" s="7"/>
       <c r="D32" s="11"/>
       <c r="F32" s="13"/>
@@ -2129,6 +2204,7 @@
   <hyperlinks>
     <hyperlink ref="G13" r:id="rId1" xr:uid="{77E0BF0A-E1F3-4143-A4CD-092E258715A6}"/>
     <hyperlink ref="G18" r:id="rId2" xr:uid="{D9AC54C5-C1D6-4646-AD7B-B2424B9949C4}"/>
+    <hyperlink ref="G22" r:id="rId3" xr:uid="{5D27E5C3-02C0-4CD7-830F-A929E4541E43}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2141,7 +2217,7 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>